<commit_message>
Code compiles; on the way to passing all tests
</commit_message>
<xml_diff>
--- a/groove/branches/aspects/src/main/resources/aspects.xlsx
+++ b/groove/branches/aspects/src/main/resources/aspects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2023-03\groove\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2022-09\aspects\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C0875B-5D66-4848-9E26-578048C3461E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D8C92-36C8-4FC1-B7C9-32183CAA0B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,13 +376,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="60"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -391,12 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="60"/>
     </xf>
@@ -407,9 +397,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -698,18 +685,18 @@
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="9" width="6.140625" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" customWidth="1"/>
     <col min="12" max="17" width="6.140625" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="2"/>
-    <col min="20" max="20" width="9.140625" style="17"/>
+    <col min="20" max="20" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -725,9 +712,9 @@
       <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="18"/>
+      <c r="J1" s="8"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="12"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -748,35 +735,35 @@
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="18"/>
+      <c r="J2" s="8"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="12"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="18"/>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="12"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -792,7 +779,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="6"/>
+      <c r="J4" s="5"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -817,7 +804,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="6"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -848,7 +835,7 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="6"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -877,7 +864,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="6"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -902,7 +889,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="6"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -925,7 +912,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="6"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -950,7 +937,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="6"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -977,7 +964,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="6"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1002,7 +989,7 @@
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="6"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1025,7 +1012,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="6"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1048,7 +1035,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="6"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1071,7 +1058,7 @@
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="6"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1094,7 +1081,7 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1112,7 +1099,7 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="6"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1143,10 +1130,10 @@
         <v>6</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="4" t="s">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -1164,7 +1151,7 @@
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1178,7 +1165,7 @@
       <c r="K21" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="10"/>
+      <c r="L21" s="7"/>
       <c r="M21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1192,11 +1179,11 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="6" t="str">
+      <c r="B22" s="5" t="str">
         <f>C21</f>
         <v>-</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1207,11 +1194,11 @@
       <c r="K22" t="s">
         <v>3</v>
       </c>
-      <c r="L22" s="6" t="str">
+      <c r="L22" s="5" t="str">
         <f>M21</f>
         <v>-</v>
       </c>
-      <c r="M22" s="10"/>
+      <c r="M22" s="7"/>
       <c r="N22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1222,31 +1209,31 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="6" t="str">
+      <c r="B23" s="5" t="str">
         <f>D21</f>
         <v>-</v>
       </c>
-      <c r="C23" s="6" t="str">
+      <c r="C23" s="5" t="str">
         <f>D22</f>
         <v>-</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="9" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2"/>
       <c r="K23" t="s">
         <v>5</v>
       </c>
-      <c r="L23" s="6" t="str">
+      <c r="L23" s="5" t="str">
         <f>N21</f>
         <v>-</v>
       </c>
-      <c r="M23" s="6" t="str">
+      <c r="M23" s="5" t="str">
         <f>N22</f>
         <v>-</v>
       </c>
-      <c r="N23" s="10"/>
+      <c r="N23" s="7"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
@@ -1254,34 +1241,32 @@
       <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="6" t="str">
+      <c r="B24" s="5" t="str">
         <f>E21</f>
         <v>-</v>
       </c>
-      <c r="C24" s="6" t="str">
+      <c r="C24" s="5" t="str">
         <f>E22</f>
         <v>-</v>
       </c>
-      <c r="D24" s="6" t="str">
+      <c r="D24" s="5" t="str">
         <f>E23</f>
         <v>X</v>
       </c>
-      <c r="E24" s="10"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="2"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1333,8 +1318,8 @@
       <c r="I28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="4" t="s">
+      <c r="J28" s="9"/>
+      <c r="K28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L28" s="3" t="s">
@@ -1360,43 +1345,43 @@
       <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J29" s="16"/>
+      <c r="D29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="10"/>
       <c r="K29" t="s">
         <v>25</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="N29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="O29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="P29" s="9" t="s">
+      <c r="L29" s="7"/>
+      <c r="M29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Q29" s="2" t="s">
@@ -1405,7 +1390,7 @@
       <c r="S29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T29" s="17" t="s">
+      <c r="T29" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1413,54 +1398,54 @@
       <c r="A30" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="6" t="str">
+      <c r="B30" s="5" t="str">
         <f>C29</f>
         <v>-</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="9" t="s">
+      <c r="G30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J30" s="16"/>
+      <c r="J30" s="10"/>
       <c r="K30" t="s">
         <v>0</v>
       </c>
-      <c r="L30" s="6" t="str">
+      <c r="L30" s="5" t="str">
         <f>M29</f>
         <v>-</v>
       </c>
-      <c r="M30" s="10"/>
-      <c r="N30" s="9" t="s">
+      <c r="M30" s="7"/>
+      <c r="N30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="O30" s="9" t="s">
+      <c r="O30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="P30" s="9" t="s">
+      <c r="P30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Q30" s="9" t="s">
+      <c r="Q30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T30" s="17" t="s">
+      <c r="T30" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1468,22 +1453,22 @@
       <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="6" t="str">
+      <c r="B31" s="5" t="str">
         <f>D29</f>
         <v>-</v>
       </c>
-      <c r="C31" s="6" t="str">
+      <c r="C31" s="5" t="str">
         <f>D30</f>
         <v>-</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -1492,32 +1477,32 @@
       <c r="I31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="6"/>
+      <c r="J31" s="5"/>
       <c r="K31" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="6" t="str">
+      <c r="L31" s="5" t="str">
         <f>N29</f>
         <v>-</v>
       </c>
-      <c r="M31" s="6" t="str">
+      <c r="M31" s="5" t="str">
         <f>N30</f>
         <v>c6</v>
       </c>
-      <c r="N31" s="10"/>
+      <c r="N31" s="7"/>
       <c r="O31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q31" s="9" t="s">
+      <c r="Q31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T31" s="17" t="s">
+      <c r="T31" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1525,48 +1510,48 @@
       <c r="A32" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="6" t="str">
+      <c r="B32" s="5" t="str">
         <f>E29</f>
         <v>-</v>
       </c>
-      <c r="C32" s="6" t="str">
+      <c r="C32" s="5" t="str">
         <f>E30</f>
         <v>c1</v>
       </c>
-      <c r="D32" s="6" t="str">
+      <c r="D32" s="5" t="str">
         <f>E31</f>
         <v>-</v>
       </c>
-      <c r="E32" s="10"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="9" t="s">
+      <c r="G32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="6"/>
+      <c r="J32" s="5"/>
       <c r="K32" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="6" t="str">
+      <c r="L32" s="5" t="str">
         <f>O29</f>
         <v>-</v>
       </c>
-      <c r="M32" s="6" t="str">
+      <c r="M32" s="5" t="str">
         <f>O30</f>
         <v>c1</v>
       </c>
-      <c r="N32" s="6" t="str">
+      <c r="N32" s="5" t="str">
         <f>O31</f>
         <v>-</v>
       </c>
-      <c r="O32" s="10"/>
+      <c r="O32" s="7"/>
       <c r="P32" s="2" t="s">
         <v>33</v>
       </c>
@@ -1576,7 +1561,7 @@
       <c r="S32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T32" s="17" t="s">
+      <c r="T32" s="11" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1584,23 +1569,23 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="6" t="str">
+      <c r="B33" s="5" t="str">
         <f>F29</f>
         <v>-</v>
       </c>
-      <c r="C33" s="6" t="str">
+      <c r="C33" s="5" t="str">
         <f>F30</f>
         <v>c1</v>
       </c>
-      <c r="D33" s="6" t="str">
+      <c r="D33" s="5" t="str">
         <f>F31</f>
         <v>-</v>
       </c>
-      <c r="E33" s="6" t="str">
+      <c r="E33" s="5" t="str">
         <f>F32</f>
         <v>-</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1610,34 +1595,34 @@
       <c r="I33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J33" s="6"/>
+      <c r="J33" s="5"/>
       <c r="K33" t="s">
         <v>3</v>
       </c>
-      <c r="L33" s="6" t="str">
+      <c r="L33" s="5" t="str">
         <f>P29</f>
         <v>-</v>
       </c>
-      <c r="M33" s="6" t="str">
+      <c r="M33" s="5" t="str">
         <f>P30</f>
         <v>c1</v>
       </c>
-      <c r="N33" s="6" t="str">
+      <c r="N33" s="5" t="str">
         <f>P31</f>
         <v>-</v>
       </c>
-      <c r="O33" s="6" t="str">
+      <c r="O33" s="5" t="str">
         <f>P32</f>
         <v>-</v>
       </c>
-      <c r="P33" s="10"/>
+      <c r="P33" s="7"/>
       <c r="Q33" s="2" t="s">
         <v>33</v>
       </c>
       <c r="S33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T33" s="17" t="s">
+      <c r="T33" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1645,62 +1630,62 @@
       <c r="A34" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="6" t="str">
+      <c r="B34" s="5" t="str">
         <f>G29</f>
         <v>-</v>
       </c>
-      <c r="C34" s="6" t="str">
+      <c r="C34" s="5" t="str">
         <f>G30</f>
         <v>X</v>
       </c>
-      <c r="D34" s="6" t="str">
+      <c r="D34" s="5" t="str">
         <f>G31</f>
         <v>c5</v>
       </c>
-      <c r="E34" s="6" t="str">
+      <c r="E34" s="5" t="str">
         <f>G32</f>
         <v>X</v>
       </c>
-      <c r="F34" s="6" t="str">
+      <c r="F34" s="5" t="str">
         <f>G33</f>
         <v>-</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="16"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="10"/>
       <c r="K34" t="s">
         <v>5</v>
       </c>
-      <c r="L34" s="6" t="str">
+      <c r="L34" s="5" t="str">
         <f>Q29</f>
         <v>-</v>
       </c>
-      <c r="M34" s="6" t="str">
+      <c r="M34" s="5" t="str">
         <f>Q30</f>
         <v>c4</v>
       </c>
-      <c r="N34" s="6" t="str">
+      <c r="N34" s="5" t="str">
         <f>Q31</f>
         <v>X</v>
       </c>
-      <c r="O34" s="6" t="str">
+      <c r="O34" s="5" t="str">
         <f>Q32</f>
         <v>-</v>
       </c>
-      <c r="P34" s="6" t="str">
+      <c r="P34" s="5" t="str">
         <f>Q33</f>
         <v>-</v>
       </c>
-      <c r="Q34" s="10"/>
+      <c r="Q34" s="7"/>
       <c r="S34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T34" s="17" t="s">
+      <c r="T34" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1708,35 +1693,35 @@
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="6" t="str">
+      <c r="B35" s="5" t="str">
         <f>H29</f>
         <v>-</v>
       </c>
-      <c r="C35" s="6" t="str">
+      <c r="C35" s="5" t="str">
         <f>H30</f>
         <v>c2</v>
       </c>
-      <c r="D35" s="6" t="str">
+      <c r="D35" s="5" t="str">
         <f>H31</f>
         <v>-</v>
       </c>
-      <c r="E35" s="6" t="str">
+      <c r="E35" s="5" t="str">
         <f>H32</f>
         <v>X</v>
       </c>
-      <c r="F35" s="6" t="str">
+      <c r="F35" s="5" t="str">
         <f>H33</f>
         <v>-</v>
       </c>
-      <c r="G35" s="6" t="str">
+      <c r="G35" s="5" t="str">
         <f>H34</f>
         <v>X</v>
       </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="16"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="10"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -1748,36 +1733,36 @@
       <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="6" t="str">
+      <c r="B36" s="5" t="str">
         <f>I29</f>
         <v>-</v>
       </c>
-      <c r="C36" s="6" t="str">
+      <c r="C36" s="5" t="str">
         <f>I30</f>
         <v>c3</v>
       </c>
-      <c r="D36" s="6" t="str">
+      <c r="D36" s="5" t="str">
         <f>I31</f>
         <v>-</v>
       </c>
-      <c r="E36" s="6" t="str">
+      <c r="E36" s="5" t="str">
         <f>I32</f>
         <v>-</v>
       </c>
-      <c r="F36" s="6" t="str">
+      <c r="F36" s="5" t="str">
         <f>I33</f>
         <v>-</v>
       </c>
-      <c r="G36" s="6" t="str">
+      <c r="G36" s="5" t="str">
         <f>I34</f>
         <v>X</v>
       </c>
-      <c r="H36" s="6" t="str">
+      <c r="H36" s="5" t="str">
         <f>I35</f>
         <v>X</v>
       </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="6"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="5"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -1785,17 +1770,15 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="6"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="19"/>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1826,8 +1809,8 @@
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="4" t="s">
+      <c r="J39" s="9"/>
+      <c r="K39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -1851,7 +1834,7 @@
       <c r="A40" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="2" t="s">
         <v>33</v>
       </c>
@@ -1869,11 +1852,11 @@
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="6"/>
+      <c r="J40" s="5"/>
       <c r="K40" t="s">
         <v>25</v>
       </c>
-      <c r="L40" s="10"/>
+      <c r="L40" s="7"/>
       <c r="M40" s="2" t="s">
         <v>33</v>
       </c>
@@ -1890,7 +1873,7 @@
       <c r="S40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T40" s="17" t="s">
+      <c r="T40" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1898,11 +1881,11 @@
       <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="6" t="str">
+      <c r="B41" s="5" t="str">
         <f>C40</f>
         <v>-</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="2" t="s">
         <v>33</v>
       </c>
@@ -1917,19 +1900,19 @@
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="6"/>
+      <c r="J41" s="5"/>
       <c r="K41" t="s">
         <v>2</v>
       </c>
-      <c r="L41" s="6" t="str">
+      <c r="L41" s="5" t="str">
         <f>M40</f>
         <v>-</v>
       </c>
-      <c r="M41" s="10"/>
+      <c r="M41" s="7"/>
       <c r="N41" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O41" s="9" t="s">
+      <c r="O41" s="6" t="s">
         <v>18</v>
       </c>
       <c r="P41" s="2" t="s">
@@ -1941,43 +1924,43 @@
       <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="6" t="str">
+      <c r="B42" s="5" t="str">
         <f>D40</f>
         <v>-</v>
       </c>
-      <c r="C42" s="6" t="str">
+      <c r="C42" s="5" t="str">
         <f>D41</f>
         <v>-</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="7"/>
       <c r="E42" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="16"/>
+      <c r="G42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="10"/>
       <c r="K42" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="6" t="str">
+      <c r="L42" s="5" t="str">
         <f>N40</f>
         <v>-</v>
       </c>
-      <c r="M42" s="6" t="str">
+      <c r="M42" s="5" t="str">
         <f>N41</f>
         <v>-</v>
       </c>
-      <c r="N42" s="10"/>
-      <c r="O42" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P42" s="9" t="s">
+      <c r="N42" s="7"/>
+      <c r="O42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P42" s="6" t="s">
         <v>28</v>
       </c>
       <c r="Q42" s="2"/>
@@ -1986,45 +1969,45 @@
       <c r="A43" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="6" t="str">
+      <c r="B43" s="5" t="str">
         <f>E40</f>
         <v>-</v>
       </c>
-      <c r="C43" s="6" t="str">
+      <c r="C43" s="5" t="str">
         <f>E41</f>
         <v>-</v>
       </c>
-      <c r="D43" s="6" t="str">
+      <c r="D43" s="5" t="str">
         <f>E42</f>
         <v>-</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="9" t="s">
+      <c r="E43" s="7"/>
+      <c r="F43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="6"/>
+      <c r="J43" s="5"/>
       <c r="K43" t="s">
         <v>11</v>
       </c>
-      <c r="L43" s="6" t="str">
+      <c r="L43" s="5" t="str">
         <f>O40</f>
         <v>-</v>
       </c>
-      <c r="M43" s="6" t="str">
+      <c r="M43" s="5" t="str">
         <f>O41</f>
         <v>X</v>
       </c>
-      <c r="N43" s="6" t="str">
+      <c r="N43" s="5" t="str">
         <f>O42</f>
         <v>X</v>
       </c>
-      <c r="O43" s="10"/>
-      <c r="P43" s="9" t="s">
+      <c r="O43" s="7"/>
+      <c r="P43" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Q43" s="2"/>
@@ -2033,98 +2016,96 @@
       <c r="A44" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="6" t="str">
+      <c r="B44" s="5" t="str">
         <f>F40</f>
         <v>-</v>
       </c>
-      <c r="C44" s="6" t="str">
+      <c r="C44" s="5" t="str">
         <f>F41</f>
         <v>-</v>
       </c>
-      <c r="D44" s="6" t="str">
+      <c r="D44" s="5" t="str">
         <f>F42</f>
         <v>-</v>
       </c>
-      <c r="E44" s="6" t="str">
+      <c r="E44" s="5" t="str">
         <f>F43</f>
         <v>-</v>
       </c>
-      <c r="F44" s="10"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="6"/>
+      <c r="J44" s="5"/>
       <c r="K44" t="s">
         <v>37</v>
       </c>
-      <c r="L44" s="6" t="str">
+      <c r="L44" s="5" t="str">
         <f>P40</f>
         <v>-</v>
       </c>
-      <c r="M44" s="6" t="str">
+      <c r="M44" s="5" t="str">
         <f>P41</f>
         <v>-</v>
       </c>
-      <c r="N44" s="6" t="str">
+      <c r="N44" s="5" t="str">
         <f>P42</f>
         <v>c1</v>
       </c>
-      <c r="O44" s="6" t="str">
+      <c r="O44" s="5" t="str">
         <f>P43</f>
         <v>X</v>
       </c>
-      <c r="P44" s="10"/>
+      <c r="P44" s="7"/>
       <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="6" t="str">
+      <c r="B45" s="5" t="str">
         <f>G40</f>
         <v>-</v>
       </c>
-      <c r="C45" s="6" t="str">
+      <c r="C45" s="5" t="str">
         <f>G41</f>
         <v>-</v>
       </c>
-      <c r="D45" s="6" t="str">
+      <c r="D45" s="5" t="str">
         <f>G42</f>
         <v>X</v>
       </c>
-      <c r="E45" s="6" t="str">
+      <c r="E45" s="5" t="str">
         <f>G43</f>
         <v>-</v>
       </c>
-      <c r="F45" s="6" t="str">
+      <c r="F45" s="5" t="str">
         <f>G44</f>
         <v>-</v>
       </c>
-      <c r="G45" s="10"/>
+      <c r="G45" s="7"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
+      <c r="J45" s="5"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="6"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="5"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>

</xml_diff>

<commit_message>
More bug fixes. Maybe we can improve early aspect conflict checking in the aspect map?
</commit_message>
<xml_diff>
--- a/groove/branches/aspects/src/main/resources/aspects.xlsx
+++ b/groove/branches/aspects/src/main/resources/aspects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2022-09\aspects\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D8C92-36C8-4FC1-B7C9-32183CAA0B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B80DF-ADC1-4AF0-8046-7A45B79DCFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Category usage" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="44">
   <si>
     <t>ROLE</t>
   </si>
@@ -685,7 +685,7 @@
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,7 +1497,7 @@
         <v>33</v>
       </c>
       <c r="Q31" s="6" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>31</v>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="N34" s="5" t="str">
         <f>Q31</f>
-        <v>X</v>
+        <v>c6</v>
       </c>
       <c r="O34" s="5" t="str">
         <f>Q32</f>
@@ -1820,15 +1820,17 @@
         <v>2</v>
       </c>
       <c r="N39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O39" s="3" t="s">
+      <c r="P39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q39" s="3"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1860,7 +1862,7 @@
       <c r="M40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="N40" s="6" t="s">
         <v>33</v>
       </c>
       <c r="O40" s="2" t="s">
@@ -1869,7 +1871,9 @@
       <c r="P40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q40" s="2"/>
+      <c r="Q40" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="S40" s="2" t="s">
         <v>28</v>
       </c>
@@ -1909,16 +1913,18 @@
         <v>-</v>
       </c>
       <c r="M41" s="7"/>
-      <c r="N41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q41" s="2"/>
+      <c r="N41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1946,7 +1952,7 @@
       <c r="I42" s="6"/>
       <c r="J42" s="10"/>
       <c r="K42" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L42" s="5" t="str">
         <f>N40</f>
@@ -1961,9 +1967,11 @@
         <v>18</v>
       </c>
       <c r="P42" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q42" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1992,7 +2000,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="5"/>
       <c r="K43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L43" s="5" t="str">
         <f>O40</f>
@@ -2000,7 +2008,7 @@
       </c>
       <c r="M43" s="5" t="str">
         <f>O41</f>
-        <v>X</v>
+        <v>-</v>
       </c>
       <c r="N43" s="5" t="str">
         <f>O42</f>
@@ -2010,7 +2018,9 @@
       <c r="P43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q43" s="2"/>
+      <c r="Q43" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2040,7 +2050,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="5"/>
       <c r="K44" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="L44" s="5" t="str">
         <f>P40</f>
@@ -2048,18 +2058,20 @@
       </c>
       <c r="M44" s="5" t="str">
         <f>P41</f>
-        <v>-</v>
+        <v>X</v>
       </c>
       <c r="N44" s="5" t="str">
         <f>P42</f>
-        <v>c1</v>
+        <v>X</v>
       </c>
       <c r="O44" s="5" t="str">
         <f>P43</f>
         <v>X</v>
       </c>
       <c r="P44" s="7"/>
-      <c r="Q44" s="2"/>
+      <c r="Q44" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2089,12 +2101,30 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="5"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
+      <c r="K45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" s="5" t="str">
+        <f>Q40</f>
+        <v>-</v>
+      </c>
+      <c r="M45" s="5" t="str">
+        <f>Q41</f>
+        <v>-</v>
+      </c>
+      <c r="N45" s="5" t="str">
+        <f>Q42</f>
+        <v>X</v>
+      </c>
+      <c r="O45" s="5" t="str">
+        <f>Q43</f>
+        <v>c1</v>
+      </c>
+      <c r="P45" s="5" t="str">
+        <f>Q44</f>
+        <v>X</v>
+      </c>
+      <c r="Q45" s="7"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>

</xml_diff>